<commit_message>
Add user plak m2m
</commit_message>
<xml_diff>
--- a/jahadurls.xlsx
+++ b/jahadurls.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="78">
   <si>
     <t xml:space="preserve">مسیر</t>
   </si>
@@ -85,6 +85,171 @@
     <t xml:space="preserve">لیست همه شهرستان ها</t>
   </si>
   <si>
+    <t xml:space="preserve">/api/auth/apis/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isAdmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لیست همه دسترسی ها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ساخت دسترسی جدید</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/auth/apis/ (api id) /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">گرفتن یک دسترسی مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ویرایش یک دسترسی مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حذف یک دسترسی مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/auth/tools/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لیست همه ابزار ها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ساخت ابزار جدید</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/auth/tools/ (tool id) /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">گرفتن یک ابزار مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ویرایش یک ابزار مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حذف یک ابزار مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/auth/roles/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لیست همه نقش ها</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/api/auth/roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ساخت نقش جدید</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/api/auth/roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/ (role id) /</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">گرفتن یک نقش مشخص</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/api/auth/roles/ (role</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> id) /</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ویرایش یک نقش مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حذف یک نقش مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/auth/usermanagement/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لیست همه کاربرهای موجود در سامانه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ساخت یک کاربر جدید </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/auth/userprofile/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">گرفتن اطلاعات کاربر توسط خوده کاربر بعد از لاگین موفق</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Noto Sans Arabic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ویرایش اطلاعات کاربر توسط خوده کاربر
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(شامل دسترسی ها نمیشود فقط firstname , lastname , ....)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">/api/common/company/</t>
   </si>
   <si>
@@ -103,13 +268,7 @@
     <t xml:space="preserve">گرفتن مشخصات یک شرکت</t>
   </si>
   <si>
-    <t xml:space="preserve">PUT</t>
-  </si>
-  <si>
     <t xml:space="preserve">اپدیت مشخصات یک شرکت</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DELETE</t>
   </si>
   <si>
     <t xml:space="preserve">حذف یک شرکت</t>
@@ -182,6 +341,42 @@
   <si>
     <t xml:space="preserve">حذف کامل یک لایه کاداستری قدیمی</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/api/landreg/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">updatecadasterstatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/(cadasterid)/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">تغییر وضعیت یک کاداستر مشخص</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فقط superuser یا is_moshaver
+اجازه انجام این عملیات را دارد </t>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +385,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -266,33 +461,31 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,7 +507,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFA6A6"/>
-        <bgColor rgb="FFFF8080"/>
+        <bgColor rgb="FFFFDBB6"/>
       </patternFill>
     </fill>
     <fill>
@@ -332,13 +525,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD4EA6B"/>
-        <bgColor rgb="FFFFDE59"/>
+        <bgColor rgb="FFE8F2A1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF6D"/>
-        <bgColor rgb="FFFFDE59"/>
+        <bgColor rgb="FFE8F2A1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6D6D"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2A1"/>
+        <bgColor rgb="FFFFF5CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -395,7 +606,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,19 +683,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="2"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="2"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -492,28 +703,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -541,14 +756,14 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFD4EA6B"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF6D6D"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -561,7 +776,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFD4EA6B"/>
+      <rgbColor rgb="FFE8F2A1"/>
       <rgbColor rgb="FFFFFF6D"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFFA6A6"/>
@@ -701,8 +916,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="28.35" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -841,13 +1056,13 @@
         <f aca="false">ROW()-1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="15" t="s">
@@ -860,13 +1075,13 @@
         <f aca="false">ROW()-1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="15" t="s">
@@ -879,13 +1094,13 @@
         <f aca="false">ROW()-1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="15" t="s">
@@ -898,13 +1113,13 @@
         <f aca="false">ROW()-1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="15" t="s">
@@ -917,13 +1132,13 @@
         <f aca="false">ROW()-1</f>
         <v>10</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="15" t="s">
@@ -932,172 +1147,526 @@
       <c r="F11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
+      <c r="A12" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="24" t="s">
+      <c r="E13" s="15" t="s">
         <v>33</v>
       </c>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="25" t="s">
+      <c r="A15" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>14</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>15</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="25" t="s">
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>16</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>38</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
-      <c r="B17" s="28" t="s">
-        <v>41</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>17</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>18</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="C19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
-      <c r="B18" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="13" t="s">
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>19</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D21" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="26"/>
-    </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="26"/>
-    </row>
-    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
-      <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
+      <c r="E21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="B22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="D22" s="0"/>
-      <c r="E22" s="0"/>
-      <c r="F22" s="0"/>
-      <c r="G22" s="0"/>
-    </row>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6"/>
+      <c r="B23" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>23</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>24</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>25</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>26</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="16"/>
+    </row>
+    <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>27</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>28</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="n">
+        <f aca="false">ROW()-1</f>
+        <v>29</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+    </row>
+    <row r="32" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="26"/>
+    </row>
+    <row r="34" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
     <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1140,7 +1709,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A31:F31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>